<commit_message>
Push code test 24022021
</commit_message>
<xml_diff>
--- a/data/DocProTestData.xlsx
+++ b/data/DocProTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="TC001to5" sheetId="1" r:id="rId1"/>
@@ -821,7 +821,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -911,7 +911,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -929,7 +929,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -970,7 +970,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -1269,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>

</xml_diff>